<commit_message>
implement the functions for splitting the table according to some special requirements
</commit_message>
<xml_diff>
--- a/MyLab/JS-HtmlTableToXLSX-01/TestCase01.xlsx
+++ b/MyLab/JS-HtmlTableToXLSX-01/TestCase01.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>header1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -273,6 +273,84 @@
   </si>
   <si>
     <t>member11</t>
+  </si>
+  <si>
+    <t>prop1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prop1-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prop1-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prop1-03</t>
+  </si>
+  <si>
+    <t>prop1-04</t>
+  </si>
+  <si>
+    <t>prop1-05</t>
+  </si>
+  <si>
+    <t>prop1-06</t>
+  </si>
+  <si>
+    <t>prop1-07</t>
+  </si>
+  <si>
+    <t>prop1-08</t>
+  </si>
+  <si>
+    <t>prop1-09</t>
+  </si>
+  <si>
+    <t>prop1-10</t>
+  </si>
+  <si>
+    <t>prop1-11</t>
+  </si>
+  <si>
+    <t>prop2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prop2-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prop2-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prop2-03</t>
+  </si>
+  <si>
+    <t>prop2-04</t>
+  </si>
+  <si>
+    <t>prop2-05</t>
+  </si>
+  <si>
+    <t>prop2-06</t>
+  </si>
+  <si>
+    <t>prop2-07</t>
+  </si>
+  <si>
+    <t>prop2-08</t>
+  </si>
+  <si>
+    <t>prop2-09</t>
+  </si>
+  <si>
+    <t>prop2-10</t>
+  </si>
+  <si>
+    <t>prop2-11</t>
   </si>
 </sst>
 </file>
@@ -649,251 +727,323 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE12"/>
+  <dimension ref="A1:AG12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>50</v>
       </c>
       <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>27</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>28</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>29</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>30</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>31</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>32</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>33</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>35</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>36</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>60</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>61</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>62</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>63</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:33">
       <c r="A2" t="s">
         <v>51</v>
       </c>
       <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:33">
       <c r="A3" t="s">
         <v>52</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:33">
       <c r="A4" t="s">
         <v>53</v>
       </c>
-      <c r="G4" t="s">
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" t="s">
         <v>18</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:33">
       <c r="A5" t="s">
         <v>54</v>
       </c>
-      <c r="I5" t="s">
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" t="s">
         <v>16</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>17</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:33">
       <c r="A6" t="s">
         <v>55</v>
       </c>
-      <c r="L6" t="s">
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+      <c r="N6" t="s">
         <v>13</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:33">
       <c r="A7" t="s">
         <v>56</v>
       </c>
-      <c r="N7" t="s">
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="P7" t="s">
         <v>37</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>38</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>39</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="S7" t="s">
         <v>40</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:33">
       <c r="A8" t="s">
         <v>57</v>
       </c>
-      <c r="S8" t="s">
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="U8" t="s">
         <v>42</v>
       </c>
-      <c r="T8" t="s">
+      <c r="V8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:33">
       <c r="A9" t="s">
         <v>58</v>
       </c>
-      <c r="U9" t="s">
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+      <c r="W9" t="s">
         <v>44</v>
       </c>
-      <c r="V9" t="s">
+      <c r="X9" t="s">
         <v>45</v>
       </c>
-      <c r="W9" t="s">
+      <c r="Y9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:33">
       <c r="A10" t="s">
         <v>59</v>
       </c>
-      <c r="X10" t="s">
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z10" t="s">
         <v>47</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="AA10" t="s">
         <v>48</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AB10" t="s">
         <v>49</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AC10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:33">
       <c r="A11" t="s">
         <v>70</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD11" t="s">
         <v>66</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AE11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:33">
       <c r="A12" t="s">
         <v>71</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF12" t="s">
         <v>68</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AG12" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>